<commit_message>
add login captcha breaker
</commit_message>
<xml_diff>
--- a/work_form/work.xlsx
+++ b/work_form/work.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9FDB18-8D1D-4618-B9F8-8E5BD2AD30A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED32D4-14A6-4B40-B586-EEEED56DF063}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -411,16 +411,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -428,16 +428,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -445,16 +445,16 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -510,13 +510,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -527,13 +527,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -544,13 +544,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>

</xml_diff>